<commit_message>
change in Bug 2 added
</commit_message>
<xml_diff>
--- a/BozhanaMihaylova/Lesson 8/Bug_PSB2_restricted possibility to signin.xlsx
+++ b/BozhanaMihaylova/Lesson 8/Bug_PSB2_restricted possibility to signin.xlsx
@@ -228,6 +228,16 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -242,16 +252,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,24 +612,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -637,7 +637,7 @@
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -645,7 +645,7 @@
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
     </row>
@@ -653,65 +653,65 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="9">
-        <v>1</v>
+      <c r="B7" s="4">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="10"/>
+      <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -719,7 +719,7 @@
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -727,7 +727,7 @@
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -735,13 +735,13 @@
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -749,7 +749,7 @@
       <c r="A21" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -757,13 +757,13 @@
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -771,13 +771,13 @@
       <c r="A24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="7"/>
+      <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -785,7 +785,7 @@
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -793,7 +793,7 @@
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>